<commit_message>
Add log control and new parameters
</commit_message>
<xml_diff>
--- a/config/fund.xlsx
+++ b/config/fund.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I542388\Documents\private\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F57D520-9976-487F-8DA8-C9EFDAF2DA09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC28124-D078-4BD7-94E2-DD3BADF94D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,6 +108,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,7 +380,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,5 +431,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B5 B1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>